<commit_message>
Added some more code to do timing analysis and found that the dynamic_cast command was really slow and was adding a significant time impact to my main processing loop. I refactored some stuff to eliminate these calls in the processing loop. Helped a bit.
</commit_message>
<xml_diff>
--- a/Libraries/AnimatTesting/TestProjects/PerformanceTests/PerformaceDropBoxes.xlsx
+++ b/Libraries/AnimatTesting/TestProjects/PerformanceTests/PerformaceDropBoxes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="20730" windowHeight="11700" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Standalone</t>
   </si>
@@ -51,10 +51,76 @@
     <t>Animat</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Test plane and box. </t>
+    <t>Animat Total</t>
+  </si>
+  <si>
+    <t>Animat Test with 90 boxes. No Animat::StepSim. Progressively add items back</t>
+  </si>
+  <si>
+    <t>No AnimatStepSim</t>
+  </si>
+  <si>
+    <t>External Stim</t>
+  </si>
+  <si>
+    <t>Data Charts</t>
+  </si>
+  <si>
+    <t>Sim Recorder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neural </t>
+  </si>
+  <si>
+    <t>Physics</t>
+  </si>
+  <si>
+    <t>Definetly within AnimatSim::StepPhyscis. Progressively Add things back to that method.</t>
+  </si>
+  <si>
+    <t>RecordVideoFrame</t>
+  </si>
+  <si>
+    <t>Adapters</t>
+  </si>
+  <si>
+    <t>Structure-&gt;Step</t>
+  </si>
+  <si>
+    <t>Within Structure-&gt;Step. Add things back to it.</t>
+  </si>
+  <si>
+    <t>StepSimulation</t>
+  </si>
+  <si>
+    <t>UpdateData</t>
+  </si>
+  <si>
+    <t>Within Body::StepSim</t>
+  </si>
+  <si>
+    <t>Remove Update Data</t>
+  </si>
+  <si>
+    <t>Definetly within Body::UpdateData</t>
+  </si>
+  <si>
+    <t>Remove  Physics_UpdateAbsolutePosition</t>
+  </si>
+  <si>
+    <t>Remove Sensor::WorlMatrixUpdate</t>
+  </si>
+  <si>
+    <t>And collect of other data</t>
+  </si>
+  <si>
+    <t>Remove just UpdateWorldMatrix</t>
+  </si>
+  <si>
+    <t>Remove just the dynamic cast code in GetParentWorldMatrix</t>
+  </si>
+  <si>
+    <t>Removed dynamics casts from within processing loop</t>
   </si>
 </sst>
 </file>
@@ -132,63 +198,26 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$H$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Standalone</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+          </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$F$9:$F$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>90</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
               <c:f>Sheet2!$G$9:$G$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1.0786462E-8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.3254419999999999E-8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.3021300000000005E-8</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.6347879999999994E-8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.7939280000000003E-8</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="1"/>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet2!$F$9:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -217,19 +246,158 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1.4489280000000001E-9</c:v>
+                  <c:v>6.9013739999999996E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.5400980000000001E-8</c:v>
+                  <c:v>1.3031539999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.1286180000000004E-8</c:v>
+                  <c:v>2.2315559999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2751759999999991E-8</c:v>
+                  <c:v>2.6239380000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.1910439999999998E-8</c:v>
+                  <c:v>3.23775E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$I$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Animat</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$G$9:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$I$9:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.9986620000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4814580000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9870899999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.7916479999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5350320000000003E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$J$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Animat Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$J$9:$J$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6.5306659999999993E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9003519999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6555160000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.7465800000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.7822940000000002E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$K$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$K$9:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="4" formatCode="0.00E+00">
+                  <c:v>3.5528480000000004E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -244,11 +412,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="77057024"/>
-        <c:axId val="77064448"/>
+        <c:axId val="117589120"/>
+        <c:axId val="117590656"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="77057024"/>
+        <c:axId val="117589120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -258,7 +426,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77064448"/>
+        <c:crossAx val="117590656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -266,18 +434,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77064448"/>
+        <c:axId val="117590656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77057024"/>
+        <c:crossAx val="117589120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -303,16 +471,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>72259</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>175391</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>351658</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>175390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>131379</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>61091</xdr:rowOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>101599</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>177799</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -703,22 +871,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:R71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Y16" sqref="Y16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
-    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -731,463 +901,894 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
       <c r="B2" s="1">
-        <v>9.8384100000000001E-9</v>
+        <v>6.8005300000000004E-5</v>
       </c>
       <c r="C2" s="1">
-        <v>1.3416E-9</v>
-      </c>
-      <c r="F2">
+        <v>5.0631699999999998E-5</v>
+      </c>
+      <c r="D2" s="1">
+        <v>6.5811999999999999E-5</v>
+      </c>
+      <c r="G2">
         <v>10</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <f>AVERAGE(B2:B6)</f>
-        <v>1.0786462E-8</v>
-      </c>
-      <c r="H2">
+        <v>6.9013739999999996E-5</v>
+      </c>
+      <c r="I2">
         <f>STDEVA(B2:B6)</f>
-        <v>8.6853423520319552E-10</v>
-      </c>
-      <c r="J2" s="1">
+        <v>4.3732171353592749E-6</v>
+      </c>
+      <c r="K2" s="1">
         <f>AVERAGE(C2:C6)</f>
-        <v>1.4489280000000001E-9</v>
-      </c>
-      <c r="K2">
+        <v>4.9986620000000002E-5</v>
+      </c>
+      <c r="L2">
         <f>STDEVA(C2:C6)</f>
-        <v>7.483087277320766E-11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2.6378564151598552E-6</v>
+      </c>
+      <c r="N2" s="1">
+        <f>AVERAGE(D2:D6)</f>
+        <v>6.5306659999999993E-5</v>
+      </c>
+      <c r="O2">
+        <f>STDEVA(D2:D6)</f>
+        <v>2.873436060363969E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
       <c r="B3" s="1">
-        <v>1.20744E-8</v>
+        <v>6.71073E-5</v>
       </c>
       <c r="C3" s="1">
-        <v>1.5204799999999999E-9</v>
-      </c>
-      <c r="F3">
+        <v>4.96249E-5</v>
+      </c>
+      <c r="D3" s="1">
+        <v>6.5069900000000005E-5</v>
+      </c>
+      <c r="G3">
         <v>30</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <f>AVERAGE(B7:B11)</f>
-        <v>2.3254419999999999E-8</v>
-      </c>
-      <c r="H3">
+        <v>1.3031539999999999E-4</v>
+      </c>
+      <c r="I3">
         <f>STDEVA(B7:B11)</f>
-        <v>7.7713693259296311E-10</v>
-      </c>
-      <c r="J3" s="1">
+        <v>1.1370736972597687E-5</v>
+      </c>
+      <c r="K3" s="1">
         <f>AVERAGE(C7:C11)</f>
-        <v>2.5400980000000001E-8</v>
-      </c>
-      <c r="K3">
+        <v>1.4814580000000003E-4</v>
+      </c>
+      <c r="L3">
         <f>STDEVA(C7:C11)</f>
-        <v>7.9245565617263331E-10</v>
-      </c>
-      <c r="M3" s="1">
+        <v>5.8692630883271908E-6</v>
+      </c>
+      <c r="N3" s="1">
         <f>AVERAGE(D7:D11)</f>
-        <v>1.9140199999999999E-8</v>
-      </c>
-      <c r="N3">
+        <v>1.9003519999999998E-4</v>
+      </c>
+      <c r="O3">
         <f>STDEVA(D7:D11)</f>
-        <v>1.0372614545041188E-9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+        <v>5.9839063913132857E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
       <c r="B4" s="1">
-        <v>1.02856E-8</v>
+        <v>6.9592300000000001E-5</v>
       </c>
       <c r="C4" s="1">
-        <v>1.4310400000000001E-9</v>
-      </c>
-      <c r="F4">
+        <v>5.2841399999999999E-5</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6.8519300000000007E-5</v>
+      </c>
+      <c r="G4">
         <v>50</v>
       </c>
-      <c r="G4" s="1">
+      <c r="H4" s="1">
         <f>AVERAGE(B12:B16)</f>
-        <v>3.3021300000000005E-8</v>
-      </c>
-      <c r="H4">
+        <v>2.2315559999999999E-4</v>
+      </c>
+      <c r="I4">
         <f>STDEVA(B12:B16)</f>
-        <v>1.6533100601520575E-9</v>
-      </c>
-      <c r="J4" s="1">
+        <v>1.2306950446800373E-5</v>
+      </c>
+      <c r="K4" s="1">
         <f>AVERAGE(C12:C16)</f>
-        <v>3.1286180000000004E-8</v>
-      </c>
-      <c r="K4">
+        <v>1.9870899999999998E-4</v>
+      </c>
+      <c r="L4">
         <f>STDEVA(C12:C16)</f>
-        <v>1.1052352089035173E-9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>6.0613278248251838E-6</v>
+      </c>
+      <c r="N4" s="1">
+        <f>AVERAGE(D12:D16)</f>
+        <v>2.6555160000000003E-4</v>
+      </c>
+      <c r="O4">
+        <f>STDEVA(D12:D16)</f>
+        <v>6.3100256972535365E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>1.118E-8</v>
+        <v>7.6046399999999998E-5</v>
       </c>
       <c r="C5" s="1">
-        <v>1.5204799999999999E-9</v>
-      </c>
-      <c r="F5">
+        <v>5.1083299999999999E-5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6.6423900000000006E-5</v>
+      </c>
+      <c r="G5">
         <v>70</v>
       </c>
-      <c r="G5" s="1">
+      <c r="H5" s="1">
         <f>AVERAGE(B17:B21)</f>
-        <v>4.6347879999999994E-8</v>
-      </c>
-      <c r="H5">
+        <v>2.6239380000000004E-4</v>
+      </c>
+      <c r="I5">
         <f>STDEVA(B17:B21)</f>
-        <v>3.9136661376514985E-9</v>
-      </c>
-      <c r="J5" s="1">
+        <v>2.0950927442478526E-5</v>
+      </c>
+      <c r="K5" s="1">
         <f>AVERAGE(C17:C21)</f>
-        <v>5.2751759999999991E-8</v>
-      </c>
-      <c r="K5">
+        <v>2.7916479999999999E-4</v>
+      </c>
+      <c r="L5">
         <f>STDEVA(C17:C21)</f>
-        <v>4.0827232190046875E-9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>3.6055975510308904E-6</v>
+      </c>
+      <c r="N5" s="1">
+        <f>AVERAGE(D17:D21)</f>
+        <v>3.7465800000000004E-4</v>
+      </c>
+      <c r="O5">
+        <f>STDEVA(D17:D21)</f>
+        <v>3.8521028672661296E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
       <c r="B6" s="1">
-        <v>1.0553899999999999E-8</v>
+        <v>6.4317400000000002E-5</v>
       </c>
       <c r="C6" s="1">
-        <v>1.4310400000000001E-9</v>
-      </c>
-      <c r="F6">
+        <v>4.5751799999999998E-5</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6.0708200000000003E-5</v>
+      </c>
+      <c r="G6">
         <v>90</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <f>AVERAGE(B22:B26)</f>
-        <v>5.7939280000000003E-8</v>
-      </c>
-      <c r="H6">
+        <v>3.23775E-4</v>
+      </c>
+      <c r="I6">
         <f>STDEVA(B22:B26)</f>
-        <v>1.62279854479846E-9</v>
-      </c>
-      <c r="J6" s="1">
+        <v>2.4192519660010615E-5</v>
+      </c>
+      <c r="K6" s="1">
         <f>AVERAGE(C22:C26)</f>
-        <v>6.1910439999999998E-8</v>
-      </c>
-      <c r="K6">
+        <v>3.5350320000000003E-4</v>
+      </c>
+      <c r="L6">
         <f>STDEVA(C22:C26)</f>
-        <v>1.4796537121907963E-9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.2969628753360656E-6</v>
+      </c>
+      <c r="N6" s="1">
+        <f>AVERAGE(D22:D26)</f>
+        <v>4.7822940000000002E-4</v>
+      </c>
+      <c r="O6">
+        <f>STDEVA(D22:D26)</f>
+        <v>2.1493796314285568E-6</v>
+      </c>
+      <c r="Q6" s="1">
+        <f>AVERAGE(E22:E26)</f>
+        <v>3.5528480000000004E-4</v>
+      </c>
+      <c r="R6">
+        <f>STDEVA(E22:E26)</f>
+        <v>4.3727278900018362E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>30</v>
       </c>
       <c r="B7" s="1">
-        <v>2.20023E-8</v>
+        <v>1.1834E-4</v>
       </c>
       <c r="C7" s="1">
-        <v>2.6474299999999999E-8</v>
+        <v>1.5494900000000001E-4</v>
       </c>
       <c r="D7" s="1">
-        <v>1.8245799999999999E-8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.9710800000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
       <c r="B8" s="1">
-        <v>2.38805E-8</v>
+        <v>1.20903E-4</v>
       </c>
       <c r="C8" s="1">
-        <v>2.54904E-8</v>
+        <v>1.48221E-4</v>
       </c>
       <c r="D8" s="1">
-        <v>2.0034599999999999E-8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.9011500000000001E-4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>30</v>
       </c>
       <c r="B9" s="1">
-        <v>2.38805E-8</v>
+        <v>1.2810299999999999E-4</v>
       </c>
       <c r="C9" s="1">
-        <v>2.4327700000000002E-8</v>
+        <v>1.39567E-4</v>
       </c>
       <c r="D9" s="1">
-        <v>1.79775E-8</v>
-      </c>
-      <c r="F9">
+        <v>1.8136000000000001E-4</v>
+      </c>
+      <c r="G9">
         <v>10</v>
       </c>
-      <c r="G9">
-        <v>1.0786462E-8</v>
-      </c>
       <c r="H9" s="1">
-        <v>1.4489280000000001E-9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <f>H2</f>
+        <v>6.9013739999999996E-5</v>
+      </c>
+      <c r="I9" s="1">
+        <f>K2</f>
+        <v>4.9986620000000002E-5</v>
+      </c>
+      <c r="J9" s="1">
+        <f>N2</f>
+        <v>6.5306659999999993E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>30</v>
       </c>
       <c r="B10" s="1">
-        <v>2.3433299999999998E-8</v>
+        <v>1.4116899999999999E-4</v>
       </c>
       <c r="C10" s="1">
-        <v>2.5043199999999999E-8</v>
+        <v>1.4612699999999999E-4</v>
       </c>
       <c r="D10" s="1">
-        <v>1.9140199999999999E-8</v>
-      </c>
-      <c r="F10">
+        <v>1.8789999999999999E-4</v>
+      </c>
+      <c r="G10">
         <v>30</v>
       </c>
-      <c r="G10">
-        <v>2.3254419999999999E-8</v>
-      </c>
       <c r="H10" s="1">
-        <v>2.5400980000000001E-8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H10:H13" si="0">H3</f>
+        <v>1.3031539999999999E-4</v>
+      </c>
+      <c r="I10" s="1">
+        <f t="shared" ref="I10:I13" si="1">K3</f>
+        <v>1.4814580000000003E-4</v>
+      </c>
+      <c r="J10" s="1">
+        <f t="shared" ref="J10:J13" si="2">N3</f>
+        <v>1.9003519999999998E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>30</v>
       </c>
       <c r="B11" s="1">
-        <v>2.30755E-8</v>
+        <v>1.4306200000000001E-4</v>
       </c>
       <c r="C11" s="1">
-        <v>2.5669299999999999E-8</v>
+        <v>1.51865E-4</v>
       </c>
       <c r="D11" s="1">
-        <v>2.0302900000000001E-8</v>
-      </c>
-      <c r="F11">
+        <v>1.9369299999999999E-4</v>
+      </c>
+      <c r="G11">
         <v>50</v>
       </c>
-      <c r="G11">
-        <v>3.3021300000000005E-8</v>
-      </c>
       <c r="H11" s="1">
-        <v>3.1286180000000004E-8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2.2315559999999999E-4</v>
+      </c>
+      <c r="I11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.9870899999999998E-4</v>
+      </c>
+      <c r="J11" s="1">
+        <f t="shared" si="2"/>
+        <v>2.6555160000000003E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
       <c r="B12" s="1">
-        <v>3.4971100000000001E-8</v>
+        <v>2.1626999999999999E-4</v>
       </c>
       <c r="C12" s="1">
-        <v>3.2913999999999999E-8</v>
-      </c>
-      <c r="F12">
+        <v>1.96064E-4</v>
+      </c>
+      <c r="D12">
+        <v>2.6271399999999999E-4</v>
+      </c>
+      <c r="G12">
         <v>70</v>
       </c>
-      <c r="G12">
-        <v>4.6347879999999994E-8</v>
-      </c>
       <c r="H12" s="1">
-        <v>5.2751759999999991E-8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2.6239380000000004E-4</v>
+      </c>
+      <c r="I12" s="1">
+        <f t="shared" si="1"/>
+        <v>2.7916479999999999E-4</v>
+      </c>
+      <c r="J12" s="1">
+        <f t="shared" si="2"/>
+        <v>3.7465800000000004E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>50</v>
       </c>
       <c r="B13" s="1">
-        <v>3.2556200000000001E-8</v>
+        <v>2.2819299999999999E-4</v>
       </c>
       <c r="C13" s="1">
-        <v>3.1572400000000002E-8</v>
-      </c>
-      <c r="F13">
+        <v>2.0236000000000001E-4</v>
+      </c>
+      <c r="D13">
+        <v>2.6926400000000002E-4</v>
+      </c>
+      <c r="G13">
         <v>90</v>
       </c>
-      <c r="G13">
-        <v>5.7939280000000003E-8</v>
-      </c>
       <c r="H13" s="1">
-        <v>6.1910439999999998E-8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>3.23775E-4</v>
+      </c>
+      <c r="I13" s="1">
+        <f t="shared" si="1"/>
+        <v>3.5350320000000003E-4</v>
+      </c>
+      <c r="J13" s="1">
+        <f t="shared" si="2"/>
+        <v>4.7822940000000002E-4</v>
+      </c>
+      <c r="K13" s="1">
+        <f>Q6</f>
+        <v>3.5528480000000004E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>50</v>
       </c>
       <c r="B14" s="1">
-        <v>3.3450599999999998E-8</v>
+        <v>2.4259499999999999E-4</v>
       </c>
       <c r="C14" s="1">
-        <v>3.0051899999999998E-8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+        <v>1.9547799999999999E-4</v>
+      </c>
+      <c r="D14">
+        <v>2.6215800000000002E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>50</v>
       </c>
       <c r="B15" s="1">
-        <v>3.0499099999999999E-8</v>
+        <v>2.1483E-4</v>
       </c>
       <c r="C15" s="1">
-        <v>3.0499099999999999E-8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>2.07362E-4</v>
+      </c>
+      <c r="D15">
+        <v>2.7464500000000001E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>50</v>
       </c>
       <c r="B16" s="1">
-        <v>3.3629499999999997E-8</v>
+        <v>2.1389E-4</v>
       </c>
       <c r="C16" s="1">
-        <v>3.1393500000000002E-8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1.9228100000000001E-4</v>
+      </c>
+      <c r="D16">
+        <v>2.5897700000000002E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>70</v>
       </c>
       <c r="B17" s="2">
-        <v>4.5882799999999997E-8</v>
+        <v>2.8069E-4</v>
       </c>
       <c r="C17" s="1">
-        <v>5.2233000000000002E-8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.8093500000000001E-4</v>
+      </c>
+      <c r="D17">
+        <v>3.7721899999999998E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>70</v>
       </c>
       <c r="B18" s="1">
-        <v>4.5972200000000001E-8</v>
+        <v>2.3976999999999999E-4</v>
       </c>
       <c r="C18" s="1">
-        <v>5.2680199999999997E-8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.8456899999999998E-4</v>
+      </c>
+      <c r="D18">
+        <v>3.8005E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>70</v>
       </c>
       <c r="B19" s="2">
-        <v>4.2126299999999999E-8</v>
+        <v>2.8766499999999999E-4</v>
       </c>
       <c r="C19" s="1">
-        <v>4.9102599999999998E-8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.7642200000000002E-4</v>
+      </c>
+      <c r="D19">
+        <v>3.7148500000000001E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>70</v>
       </c>
       <c r="B20" s="1">
-        <v>4.4988400000000001E-8</v>
+        <v>2.5698300000000002E-4</v>
       </c>
       <c r="C20" s="1">
-        <v>5.01759E-8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.7802600000000001E-4</v>
+      </c>
+      <c r="D20">
+        <v>3.7332400000000002E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>70</v>
       </c>
       <c r="B21" s="1">
-        <v>5.2769699999999999E-8</v>
+        <v>2.4686100000000002E-4</v>
       </c>
       <c r="C21" s="1">
-        <v>5.9567099999999999E-8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.7587199999999998E-4</v>
+      </c>
+      <c r="D21">
+        <v>3.71212E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>90</v>
       </c>
       <c r="B22" s="1">
-        <v>5.8762099999999999E-8</v>
+        <v>3.5035399999999999E-4</v>
       </c>
       <c r="C22" s="1">
-        <v>6.0372099999999998E-8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.5328200000000001E-4</v>
+      </c>
+      <c r="D22">
+        <v>4.7740599999999999E-4</v>
+      </c>
+      <c r="E22">
+        <v>3.5624799999999998E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>90</v>
       </c>
       <c r="B23" s="1">
-        <v>5.5810600000000001E-8</v>
+        <v>3.07015E-4</v>
       </c>
       <c r="C23" s="1">
-        <v>6.1803100000000006E-8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.52555E-4</v>
+      </c>
+      <c r="D23">
+        <v>4.7686199999999999E-4</v>
+      </c>
+      <c r="E23">
+        <v>3.5757600000000002E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>90</v>
       </c>
       <c r="B24" s="1">
-        <v>5.8672700000000002E-8</v>
+        <v>3.0298199999999998E-4</v>
       </c>
       <c r="C24" s="1">
-        <v>6.4128500000000004E-8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.5533899999999998E-4</v>
+      </c>
+      <c r="D24">
+        <v>4.8181199999999997E-4</v>
+      </c>
+      <c r="E24">
+        <v>3.4839400000000003E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>90</v>
       </c>
       <c r="B25" s="1">
-        <v>5.9745999999999998E-8</v>
+        <v>3.0851099999999997E-4</v>
       </c>
       <c r="C25" s="1">
-        <v>6.08193E-8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3.5421600000000003E-4</v>
+      </c>
+      <c r="D25">
+        <v>4.7856500000000002E-4</v>
+      </c>
+      <c r="E25">
+        <v>3.5994999999999999E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>90</v>
       </c>
       <c r="B26" s="1">
-        <v>5.6704999999999997E-8</v>
+        <v>3.5001299999999998E-4</v>
       </c>
       <c r="C26" s="1">
-        <v>6.2429199999999994E-8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" t="s">
+        <v>3.5212399999999999E-4</v>
+      </c>
+      <c r="D26">
+        <v>4.7650200000000001E-4</v>
+      </c>
+      <c r="E26">
+        <v>3.54256E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36">
+        <v>3.63383E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <v>3.63937E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1">
+        <v>3.60756E-4</v>
+      </c>
+      <c r="D38" s="1"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1">
+        <v>3.6229399999999998E-4</v>
+      </c>
+      <c r="D39" s="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1">
+        <v>3.6238200000000001E-4</v>
+      </c>
+      <c r="D40" s="1"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1">
+        <v>4.9836900000000003E-4</v>
+      </c>
+      <c r="D41" s="1"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+    </row>
+    <row r="44" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>19</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1">
+        <v>3.6318500000000003E-4</v>
+      </c>
+      <c r="D45" s="1"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>21</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1">
+        <v>3.6337300000000001E-4</v>
+      </c>
+      <c r="D46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1">
+        <v>4.84716E-4</v>
+      </c>
+      <c r="D47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>25</v>
+      </c>
+      <c r="B50" s="1"/>
+      <c r="C50" s="1">
+        <v>3.6241499999999999E-4</v>
+      </c>
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1">
+        <v>4.7081E-4</v>
+      </c>
+      <c r="D51" s="1"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B52" s="1"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+      <c r="D53" s="1"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1">
+        <v>3.6952000000000003E-4</v>
+      </c>
+      <c r="D54" s="1"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57">
+        <v>4.79025E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58">
+        <v>3.7777600000000002E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59">
+        <v>3.6418000000000003E-4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>32</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61">
+        <v>4.5425199999999999E-4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>4.17031E-4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>4.0287899999999998E-4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>4.1552199999999998E-4</v>
+      </c>
+      <c r="D69">
+        <f>AVERAGE(A67:A71)</f>
+        <v>4.1218100000000002E-4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>4.0513799999999998E-4</v>
+      </c>
+      <c r="D70">
+        <f>_xlfn.STDEV.P(A67:A71)</f>
+        <v>6.8891733901826028E-6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>4.2033499999999998E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Added a check in CreateModule to verify that if we are in debug mode we are loading debug dll's and vice versa for release. 2. Fixed some of the project files for the new releaseunoptimized to point to the right path and to include debug info. 3. Fixed the file conversion system so that it adds references to the correct dll's based on debug/release version running.
</commit_message>
<xml_diff>
--- a/Libraries/AnimatTesting/TestProjects/PerformanceTests/PerformaceDropBoxes.xlsx
+++ b/Libraries/AnimatTesting/TestProjects/PerformanceTests/PerformaceDropBoxes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Standalone</t>
   </si>
@@ -121,14 +121,28 @@
   </si>
   <si>
     <t>Removed dynamics casts from within processing loop</t>
+  </si>
+  <si>
+    <t>AnimatLab Old</t>
+  </si>
+  <si>
+    <t>Animat Old</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -156,10 +170,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -200,7 +215,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$H$8</c:f>
+              <c:f>Sheet2!$I$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -217,7 +232,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$G$9:$G$13</c:f>
+              <c:f>Sheet2!$H$9:$H$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -241,7 +256,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$H$9:$H$13</c:f>
+              <c:f>Sheet2!$I$9:$I$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -269,7 +284,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$I$8</c:f>
+              <c:f>Sheet2!$J$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -286,7 +301,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet2!$G$9:$G$13</c:f>
+              <c:f>Sheet2!$H$9:$H$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -310,7 +325,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$I$9:$I$13</c:f>
+              <c:f>Sheet2!$J$9:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -338,7 +353,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$J$8</c:f>
+              <c:f>Sheet2!$K$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -355,7 +370,7 @@
           </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$J$9:$J$13</c:f>
+              <c:f>Sheet2!$K$9:$K$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
@@ -383,21 +398,41 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet2!$K$8</c:f>
+              <c:f>Sheet2!$L$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Animat Old</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+          </c:errBars>
           <c:val>
             <c:numRef>
-              <c:f>Sheet2!$K$9:$K$13</c:f>
+              <c:f>Sheet2!$L$9:$L$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="4" formatCode="0.00E+00">
-                  <c:v>3.5528480000000004E-4</c:v>
+                <c:pt idx="0">
+                  <c:v>1.119584E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1004680000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0713880000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0269920000000006E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.8156700000000009E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -412,11 +447,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="117589120"/>
-        <c:axId val="117590656"/>
+        <c:axId val="124675200"/>
+        <c:axId val="124676736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="117589120"/>
+        <c:axId val="124675200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,7 +461,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117590656"/>
+        <c:crossAx val="124676736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -434,7 +469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117590656"/>
+        <c:axId val="124676736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -445,7 +480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117589120"/>
+        <c:crossAx val="124675200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -471,13 +506,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>351658</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>175390</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>101599</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>177799</xdr:rowOff>
@@ -871,10 +906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R71"/>
+  <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="M14" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AK37" sqref="AK37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,13 +917,14 @@
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -901,26 +937,35 @@
       <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -933,35 +978,46 @@
       <c r="D2" s="1">
         <v>6.5811999999999999E-5</v>
       </c>
-      <c r="G2">
+      <c r="F2">
+        <v>1.1504E-4</v>
+      </c>
+      <c r="H2">
         <v>10</v>
       </c>
-      <c r="H2" s="1">
+      <c r="I2" s="1">
         <f>AVERAGE(B2:B6)</f>
         <v>6.9013739999999996E-5</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <f>STDEVA(B2:B6)</f>
         <v>4.3732171353592749E-6</v>
       </c>
-      <c r="K2" s="1">
+      <c r="L2" s="1">
         <f>AVERAGE(C2:C6)</f>
         <v>4.9986620000000002E-5</v>
       </c>
-      <c r="L2">
+      <c r="M2">
         <f>STDEVA(C2:C6)</f>
         <v>2.6378564151598552E-6</v>
       </c>
-      <c r="N2" s="1">
+      <c r="O2" s="1">
         <f>AVERAGE(D2:D6)</f>
         <v>6.5306659999999993E-5</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <f>STDEVA(D2:D6)</f>
         <v>2.873436060363969E-6</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R2" s="1">
+        <f>AVERAGE(F2:F6)</f>
+        <v>1.119584E-4</v>
+      </c>
+      <c r="S2">
+        <f>STDEVA(F2:F6)</f>
+        <v>2.5009626746515019E-6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>10</v>
       </c>
@@ -974,35 +1030,46 @@
       <c r="D3" s="1">
         <v>6.5069900000000005E-5</v>
       </c>
-      <c r="G3">
+      <c r="F3">
+        <v>1.1431500000000001E-4</v>
+      </c>
+      <c r="H3">
         <v>30</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <f>AVERAGE(B7:B11)</f>
         <v>1.3031539999999999E-4</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <f>STDEVA(B7:B11)</f>
         <v>1.1370736972597687E-5</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <f>AVERAGE(C7:C11)</f>
         <v>1.4814580000000003E-4</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <f>STDEVA(C7:C11)</f>
         <v>5.8692630883271908E-6</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <f>AVERAGE(D7:D11)</f>
         <v>1.9003519999999998E-4</v>
       </c>
-      <c r="O3">
+      <c r="P3">
         <f>STDEVA(D7:D11)</f>
         <v>5.9839063913132857E-6</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R3" s="1">
+        <f>AVERAGE(F7:F11)</f>
+        <v>3.1004680000000002E-4</v>
+      </c>
+      <c r="S3">
+        <f>STDEVA(F7:F11)</f>
+        <v>3.5344512586821696E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1015,35 +1082,46 @@
       <c r="D4" s="1">
         <v>6.8519300000000007E-5</v>
       </c>
-      <c r="G4">
+      <c r="F4">
+        <v>1.09883E-4</v>
+      </c>
+      <c r="H4">
         <v>50</v>
       </c>
-      <c r="H4" s="1">
+      <c r="I4" s="1">
         <f>AVERAGE(B12:B16)</f>
         <v>2.2315559999999999E-4</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <f>STDEVA(B12:B16)</f>
         <v>1.2306950446800373E-5</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <f>AVERAGE(C12:C16)</f>
         <v>1.9870899999999998E-4</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f>STDEVA(C12:C16)</f>
         <v>6.0613278248251838E-6</v>
       </c>
-      <c r="N4" s="1">
+      <c r="O4" s="1">
         <f>AVERAGE(D12:D16)</f>
         <v>2.6555160000000003E-4</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <f>STDEVA(D12:D16)</f>
         <v>6.3100256972535365E-6</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R4" s="1">
+        <f>AVERAGE(F12:F16)</f>
+        <v>5.0713880000000002E-4</v>
+      </c>
+      <c r="S4">
+        <f>STDEVA(F12:F16)</f>
+        <v>1.3869096390897299E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -1056,35 +1134,46 @@
       <c r="D5" s="1">
         <v>6.6423900000000006E-5</v>
       </c>
-      <c r="G5">
+      <c r="F5">
+        <v>1.10214E-4</v>
+      </c>
+      <c r="H5">
         <v>70</v>
       </c>
-      <c r="H5" s="1">
+      <c r="I5" s="1">
         <f>AVERAGE(B17:B21)</f>
         <v>2.6239380000000004E-4</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <f>STDEVA(B17:B21)</f>
         <v>2.0950927442478526E-5</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <f>AVERAGE(C17:C21)</f>
         <v>2.7916479999999999E-4</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f>STDEVA(C17:C21)</f>
         <v>3.6055975510308904E-6</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <f>AVERAGE(D17:D21)</f>
         <v>3.7465800000000004E-4</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <f>STDEVA(D17:D21)</f>
         <v>3.8521028672661296E-6</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="1">
+        <f>AVERAGE(F17:F21)</f>
+        <v>7.0269920000000006E-4</v>
+      </c>
+      <c r="S5">
+        <f>STDEVA(F17:F21)</f>
+        <v>1.2276812562713494E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
@@ -1097,43 +1186,46 @@
       <c r="D6" s="1">
         <v>6.0708200000000003E-5</v>
       </c>
-      <c r="G6">
+      <c r="F6">
+        <v>1.1034E-4</v>
+      </c>
+      <c r="H6">
         <v>90</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <f>AVERAGE(B22:B26)</f>
         <v>3.23775E-4</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <f>STDEVA(B22:B26)</f>
         <v>2.4192519660010615E-5</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <f>AVERAGE(C22:C26)</f>
         <v>3.5350320000000003E-4</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f>STDEVA(C22:C26)</f>
         <v>1.2969628753360656E-6</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <f>AVERAGE(D22:D26)</f>
         <v>4.7822940000000002E-4</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <f>STDEVA(D22:D26)</f>
         <v>2.1493796314285568E-6</v>
       </c>
-      <c r="Q6" s="1">
-        <f>AVERAGE(E22:E26)</f>
-        <v>3.5528480000000004E-4</v>
-      </c>
-      <c r="R6">
-        <f>STDEVA(E22:E26)</f>
-        <v>4.3727278900018362E-6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R6" s="1">
+        <f>AVERAGE(F22:F26)</f>
+        <v>8.8156700000000009E-4</v>
+      </c>
+      <c r="S6">
+        <f>STDEVA(F22:F26)</f>
+        <v>1.7806590072217636E-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>30</v>
       </c>
@@ -1146,8 +1238,11 @@
       <c r="D7" s="1">
         <v>1.9710800000000001E-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>3.0543500000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>30</v>
       </c>
@@ -1160,17 +1255,23 @@
       <c r="D8" s="1">
         <v>1.9011500000000001E-4</v>
       </c>
-      <c r="H8" t="s">
+      <c r="F8">
+        <v>3.14462E-4</v>
+      </c>
+      <c r="I8" t="s">
         <v>0</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>10</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>30</v>
       </c>
@@ -1183,23 +1284,30 @@
       <c r="D9" s="1">
         <v>1.8136000000000001E-4</v>
       </c>
-      <c r="G9">
+      <c r="F9">
+        <v>3.1084500000000002E-4</v>
+      </c>
+      <c r="H9">
         <v>10</v>
       </c>
-      <c r="H9" s="1">
-        <f>H2</f>
+      <c r="I9" s="1">
+        <f>I2</f>
         <v>6.9013739999999996E-5</v>
       </c>
-      <c r="I9" s="1">
-        <f>K2</f>
+      <c r="J9" s="1">
+        <f>L2</f>
         <v>4.9986620000000002E-5</v>
       </c>
-      <c r="J9" s="1">
-        <f>N2</f>
+      <c r="K9" s="1">
+        <f>O2</f>
         <v>6.5306659999999993E-5</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L9" s="1">
+        <f>R2</f>
+        <v>1.119584E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>30</v>
       </c>
@@ -1212,23 +1320,30 @@
       <c r="D10" s="1">
         <v>1.8789999999999999E-4</v>
       </c>
-      <c r="G10">
+      <c r="F10">
+        <v>3.11794E-4</v>
+      </c>
+      <c r="H10">
         <v>30</v>
       </c>
-      <c r="H10" s="1">
-        <f t="shared" ref="H10:H13" si="0">H3</f>
+      <c r="I10" s="1">
+        <f t="shared" ref="I10:I13" si="0">I3</f>
         <v>1.3031539999999999E-4</v>
       </c>
-      <c r="I10" s="1">
-        <f t="shared" ref="I10:I13" si="1">K3</f>
+      <c r="J10" s="1">
+        <f t="shared" ref="J10:J13" si="1">L3</f>
         <v>1.4814580000000003E-4</v>
       </c>
-      <c r="J10" s="1">
-        <f t="shared" ref="J10:J13" si="2">N3</f>
+      <c r="K10" s="1">
+        <f t="shared" ref="K10:K13" si="2">O3</f>
         <v>1.9003519999999998E-4</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L10" s="1">
+        <f t="shared" ref="L10:L13" si="3">R3</f>
+        <v>3.1004680000000002E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>30</v>
       </c>
@@ -1241,23 +1356,30 @@
       <c r="D11" s="1">
         <v>1.9369299999999999E-4</v>
       </c>
-      <c r="G11">
+      <c r="F11">
+        <v>3.0769800000000002E-4</v>
+      </c>
+      <c r="H11">
         <v>50</v>
       </c>
-      <c r="H11" s="1">
+      <c r="I11" s="1">
         <f t="shared" si="0"/>
         <v>2.2315559999999999E-4</v>
       </c>
-      <c r="I11" s="1">
+      <c r="J11" s="1">
         <f t="shared" si="1"/>
         <v>1.9870899999999998E-4</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K11" s="1">
         <f t="shared" si="2"/>
         <v>2.6555160000000003E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L11" s="1">
+        <f t="shared" si="3"/>
+        <v>5.0713880000000002E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>50</v>
       </c>
@@ -1270,23 +1392,30 @@
       <c r="D12">
         <v>2.6271399999999999E-4</v>
       </c>
-      <c r="G12">
+      <c r="F12">
+        <v>4.9709999999999999E-4</v>
+      </c>
+      <c r="H12">
         <v>70</v>
       </c>
-      <c r="H12" s="1">
+      <c r="I12" s="1">
         <f t="shared" si="0"/>
         <v>2.6239380000000004E-4</v>
       </c>
-      <c r="I12" s="1">
+      <c r="J12" s="1">
         <f t="shared" si="1"/>
         <v>2.7916479999999999E-4</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K12" s="1">
         <f t="shared" si="2"/>
         <v>3.7465800000000004E-4</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L12" s="1">
+        <f t="shared" si="3"/>
+        <v>7.0269920000000006E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>50</v>
       </c>
@@ -1299,27 +1428,30 @@
       <c r="D13">
         <v>2.6926400000000002E-4</v>
       </c>
-      <c r="G13">
+      <c r="F13">
+        <v>5.0793599999999996E-4</v>
+      </c>
+      <c r="H13">
         <v>90</v>
       </c>
-      <c r="H13" s="1">
+      <c r="I13" s="1">
         <f t="shared" si="0"/>
         <v>3.23775E-4</v>
       </c>
-      <c r="I13" s="1">
+      <c r="J13" s="1">
         <f t="shared" si="1"/>
         <v>3.5350320000000003E-4</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K13" s="1">
         <f t="shared" si="2"/>
         <v>4.7822940000000002E-4</v>
       </c>
-      <c r="K13" s="1">
-        <f>Q6</f>
-        <v>3.5528480000000004E-4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="L13" s="1">
+        <f t="shared" si="3"/>
+        <v>8.8156700000000009E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>50</v>
       </c>
@@ -1332,8 +1464,11 @@
       <c r="D14">
         <v>2.6215800000000002E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>5.0062000000000001E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>50</v>
       </c>
@@ -1346,8 +1481,11 @@
       <c r="D15">
         <v>2.7464500000000001E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="F15" s="3">
+        <v>4.99187E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>50</v>
       </c>
@@ -1360,8 +1498,11 @@
       <c r="D16">
         <v>2.5897700000000002E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>5.3085100000000004E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>70</v>
       </c>
@@ -1374,8 +1515,11 @@
       <c r="D17">
         <v>3.7721899999999998E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>7.1637700000000003E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>70</v>
       </c>
@@ -1388,8 +1532,11 @@
       <c r="D18">
         <v>3.8005E-4</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>6.9268200000000002E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>70</v>
       </c>
@@ -1402,8 +1549,11 @@
       <c r="D19">
         <v>3.7148500000000001E-4</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>6.9722100000000004E-4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>70</v>
       </c>
@@ -1416,8 +1566,11 @@
       <c r="D20">
         <v>3.7332400000000002E-4</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>7.1551999999999998E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>70</v>
       </c>
@@ -1430,8 +1583,11 @@
       <c r="D21">
         <v>3.71212E-4</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>6.91696E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>90</v>
       </c>
@@ -1447,8 +1603,11 @@
       <c r="E22">
         <v>3.5624799999999998E-4</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>8.8012699999999997E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>90</v>
       </c>
@@ -1464,8 +1623,11 @@
       <c r="E23">
         <v>3.5757600000000002E-4</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>8.8268799999999996E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>90</v>
       </c>
@@ -1481,8 +1643,11 @@
       <c r="E24">
         <v>3.4839400000000003E-4</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>8.7950500000000004E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>90</v>
       </c>
@@ -1498,8 +1663,11 @@
       <c r="E25">
         <v>3.5994999999999999E-4</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>8.8169300000000002E-4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>90</v>
       </c>
@@ -1514,6 +1682,9 @@
       </c>
       <c r="E26">
         <v>3.54256E-4</v>
+      </c>
+      <c r="F26">
+        <v>8.8382200000000004E-4</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>